<commit_message>
Improved performance and memory usage.
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Columns/InsertColumns.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Columns/InsertColumns.xlsx
@@ -495,14 +495,14 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="I3" s="4" t="s"/>
-      <x:c r="J3" s="4" t="s"/>
+      <x:c r="J3" s="1" t="s"/>
       <x:c r="K3" s="4" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="L3" s="4" t="s"/>
-      <x:c r="M3" s="4" t="s"/>
-      <x:c r="N3" s="4" t="s"/>
-      <x:c r="O3" s="4" t="s"/>
+      <x:c r="L3" s="1" t="s"/>
+      <x:c r="M3" s="1" t="s"/>
+      <x:c r="N3" s="1" t="s"/>
+      <x:c r="O3" s="1" t="s"/>
     </x:row>
     <x:row r="4" spans="1:17" s="4" customFormat="1">
       <x:c r="A4" s="4" t="s">
@@ -522,16 +522,16 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="I4" s="4" t="s"/>
-      <x:c r="J4" s="4" t="s"/>
+      <x:c r="J4" s="1" t="s"/>
       <x:c r="K4" s="4" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="L4" s="4" t="s"/>
-      <x:c r="M4" s="4" t="s"/>
-      <x:c r="N4" s="4" t="s"/>
-      <x:c r="O4" s="4" t="s"/>
-      <x:c r="P4" s="4" t="s"/>
-      <x:c r="Q4" s="4" t="s"/>
+      <x:c r="L4" s="1" t="s"/>
+      <x:c r="M4" s="1" t="s"/>
+      <x:c r="N4" s="1" t="s"/>
+      <x:c r="O4" s="1" t="s"/>
+      <x:c r="P4" s="1" t="s"/>
+      <x:c r="Q4" s="1" t="s"/>
     </x:row>
     <x:row r="5" spans="1:17">
       <x:c r="A5" s="1" t="s">

</xml_diff>

<commit_message>
Added row.RowUsed() and column.ColumnUsed()
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Columns/InsertColumns.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Columns/InsertColumns.xlsx
@@ -495,14 +495,14 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="I3" s="4" t="s"/>
-      <x:c r="J3" s="1" t="s"/>
+      <x:c r="J3" s="4" t="s"/>
       <x:c r="K3" s="4" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="L3" s="1" t="s"/>
-      <x:c r="M3" s="1" t="s"/>
-      <x:c r="N3" s="1" t="s"/>
-      <x:c r="O3" s="1" t="s"/>
+      <x:c r="L3" s="4" t="s"/>
+      <x:c r="M3" s="4" t="s"/>
+      <x:c r="N3" s="4" t="s"/>
+      <x:c r="O3" s="4" t="s"/>
     </x:row>
     <x:row r="4" spans="1:17" s="4" customFormat="1">
       <x:c r="A4" s="4" t="s">
@@ -522,16 +522,16 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="I4" s="4" t="s"/>
-      <x:c r="J4" s="1" t="s"/>
+      <x:c r="J4" s="4" t="s"/>
       <x:c r="K4" s="4" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="L4" s="1" t="s"/>
-      <x:c r="M4" s="1" t="s"/>
-      <x:c r="N4" s="1" t="s"/>
-      <x:c r="O4" s="1" t="s"/>
-      <x:c r="P4" s="1" t="s"/>
-      <x:c r="Q4" s="1" t="s"/>
+      <x:c r="L4" s="4" t="s"/>
+      <x:c r="M4" s="4" t="s"/>
+      <x:c r="N4" s="4" t="s"/>
+      <x:c r="O4" s="4" t="s"/>
+      <x:c r="P4" s="4" t="s"/>
+      <x:c r="Q4" s="4" t="s"/>
     </x:row>
     <x:row r="5" spans="1:17">
       <x:c r="A5" s="1" t="s">

</xml_diff>